<commit_message>
added CNN for TT dataset.
</commit_message>
<xml_diff>
--- a/output/DEEP_BASE.xlsx
+++ b/output/DEEP_BASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pree\Thai_SA_journal\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336D72A0-66B4-45D0-B46C-1A5D2796E6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5411272D-B12B-4F9E-A0C1-135BE6445FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="180">
   <si>
     <t>0RF</t>
   </si>
@@ -538,6 +538,42 @@
   </si>
   <si>
     <t>0.4971±0.0245</t>
+  </si>
+  <si>
+    <t>0.5198±0.0226</t>
+  </si>
+  <si>
+    <t>0.5871±0.1797</t>
+  </si>
+  <si>
+    <t>0.388±0.19</t>
+  </si>
+  <si>
+    <t>0.1955±0.0814</t>
+  </si>
+  <si>
+    <t>0.6725±0.0284</t>
+  </si>
+  <si>
+    <t>0.4303±0.0999</t>
+  </si>
+  <si>
+    <t>0.501±0.0197</t>
+  </si>
+  <si>
+    <t>0.4092±0.1335</t>
+  </si>
+  <si>
+    <t>0.4355±0.0603</t>
+  </si>
+  <si>
+    <t>0.1633±0.0932</t>
+  </si>
+  <si>
+    <t>0.6004±0.0563</t>
+  </si>
+  <si>
+    <t>0.4161±0.1084</t>
   </si>
 </sst>
 </file>
@@ -1560,7 +1596,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1618,18 +1654,42 @@
       <c r="A3" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3"/>
+      <c r="B3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G3" t="s">
+        <v>173</v>
+      </c>
+      <c r="I3" t="s">
+        <v>174</v>
+      </c>
+      <c r="J3" t="s">
+        <v>175</v>
+      </c>
+      <c r="K3" t="s">
+        <v>176</v>
+      </c>
+      <c r="L3" t="s">
+        <v>177</v>
+      </c>
+      <c r="M3" t="s">
+        <v>178</v>
+      </c>
+      <c r="N3" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">

</xml_diff>

<commit_message>
added links to the models.
</commit_message>
<xml_diff>
--- a/output/DEEP_BASE.xlsx
+++ b/output/DEEP_BASE.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pree\Thai_SA_journal\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5411272D-B12B-4F9E-A0C1-135BE6445FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F91C6E-F62A-49D0-9564-F6B9662B8373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WS" sheetId="2" r:id="rId1"/>
     <sheet name="TT" sheetId="3" r:id="rId2"/>
-    <sheet name="Detail" sheetId="1" r:id="rId3"/>
+    <sheet name="KT" sheetId="4" r:id="rId3"/>
+    <sheet name="Detail" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="180">
   <si>
     <t>0RF</t>
   </si>
@@ -1596,7 +1597,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1770,6 +1771,83 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19A0F0F-E513-4C34-BBE6-40C2E11D5D35}">
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="B2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD120"/>
   <sheetViews>

</xml_diff>

<commit_message>
added TX results for deep-based CNN and Bi-LSTM.
</commit_message>
<xml_diff>
--- a/output/DEEP_BASE.xlsx
+++ b/output/DEEP_BASE.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pree\Thai_SA_journal\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDA70EA-77B3-4D0D-B4B0-5C2067654A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1B039A-301E-4CAC-BAC2-24BEFCAAB8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7440" yWindow="1185" windowWidth="15225" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WS" sheetId="2" r:id="rId1"/>
     <sheet name="TT" sheetId="3" r:id="rId2"/>
     <sheet name="KT" sheetId="4" r:id="rId3"/>
-    <sheet name="Detail" sheetId="1" r:id="rId4"/>
+    <sheet name="TX" sheetId="5" r:id="rId4"/>
+    <sheet name="Detail" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="236">
   <si>
     <t>0RF</t>
   </si>
@@ -683,6 +684,66 @@
   </si>
   <si>
     <t>0.5231±0.0231</t>
+  </si>
+  <si>
+    <t>0.7112±0.039</t>
+  </si>
+  <si>
+    <t>0.3783±0.1164</t>
+  </si>
+  <si>
+    <t>0.7708±0.0546</t>
+  </si>
+  <si>
+    <t>0.6852±0.0614</t>
+  </si>
+  <si>
+    <t>0.6912±0.0523</t>
+  </si>
+  <si>
+    <t>0.6784±0.0622</t>
+  </si>
+  <si>
+    <t>0.6549±0.082</t>
+  </si>
+  <si>
+    <t>0.3904±0.188</t>
+  </si>
+  <si>
+    <t>0.7401±0.0688</t>
+  </si>
+  <si>
+    <t>0.6796±0.0624</t>
+  </si>
+  <si>
+    <t>0.6778±0.0296</t>
+  </si>
+  <si>
+    <t>0.2959±0.0764</t>
+  </si>
+  <si>
+    <t>0.7417±0.0396</t>
+  </si>
+  <si>
+    <t>0.6387±0.0441</t>
+  </si>
+  <si>
+    <t>0.6666±0.0302</t>
+  </si>
+  <si>
+    <t>0.6442±0.0375</t>
+  </si>
+  <si>
+    <t>0.6239±0.0397</t>
+  </si>
+  <si>
+    <t>0.2671±0.0774</t>
+  </si>
+  <si>
+    <t>0.7145±0.0494</t>
+  </si>
+  <si>
+    <t>0.6339±0.0385</t>
   </si>
 </sst>
 </file>
@@ -1562,7 +1623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D5C4ABC-024F-46B2-BF47-2362A367FE2E}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -1919,7 +1980,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="N5" sqref="A1:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2064,6 +2125,155 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8EE0488-B36D-46E6-911B-C64CBA69DD12}">
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="B2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D3" t="s">
+        <v>226</v>
+      </c>
+      <c r="E3" t="s">
+        <v>227</v>
+      </c>
+      <c r="F3" t="s">
+        <v>228</v>
+      </c>
+      <c r="G3" t="s">
+        <v>229</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" t="s">
+        <v>230</v>
+      </c>
+      <c r="J3" t="s">
+        <v>231</v>
+      </c>
+      <c r="K3" t="s">
+        <v>232</v>
+      </c>
+      <c r="L3" t="s">
+        <v>233</v>
+      </c>
+      <c r="M3" t="s">
+        <v>234</v>
+      </c>
+      <c r="N3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C4" t="s">
+        <v>216</v>
+      </c>
+      <c r="D4" t="s">
+        <v>216</v>
+      </c>
+      <c r="E4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F4" t="s">
+        <v>218</v>
+      </c>
+      <c r="G4" t="s">
+        <v>219</v>
+      </c>
+      <c r="I4" t="s">
+        <v>220</v>
+      </c>
+      <c r="J4" t="s">
+        <v>221</v>
+      </c>
+      <c r="K4" t="s">
+        <v>222</v>
+      </c>
+      <c r="L4" t="s">
+        <v>223</v>
+      </c>
+      <c r="M4" t="s">
+        <v>224</v>
+      </c>
+      <c r="N4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD120"/>
   <sheetViews>

</xml_diff>

<commit_message>
added BERT-TX results multilang.
</commit_message>
<xml_diff>
--- a/output/DEEP_BASE.xlsx
+++ b/output/DEEP_BASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pree\Thai_SA_journal\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1B039A-301E-4CAC-BAC2-24BEFCAAB8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B60B41-C3D6-424B-BC3A-2A714E433142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="246">
   <si>
     <t>0RF</t>
   </si>
@@ -744,6 +744,36 @@
   </si>
   <si>
     <t>0.6339±0.0385</t>
+  </si>
+  <si>
+    <t>BERT-MULT</t>
+  </si>
+  <si>
+    <t>0.6305±0.015</t>
+  </si>
+  <si>
+    <t>0.1352±0.0554</t>
+  </si>
+  <si>
+    <t>0.669±0.0133</t>
+  </si>
+  <si>
+    <t>0.4638±0.0403</t>
+  </si>
+  <si>
+    <t>0.626±0.0108</t>
+  </si>
+  <si>
+    <t>0.6466±0.0515</t>
+  </si>
+  <si>
+    <t>0.5235±0.0145</t>
+  </si>
+  <si>
+    <t>0.114±0.0477</t>
+  </si>
+  <si>
+    <t>0.578±0.0258</t>
   </si>
 </sst>
 </file>
@@ -2129,10 +2159,13 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="O5" sqref="A5:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
@@ -2265,7 +2298,43 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
-        <v>142</v>
+        <v>236</v>
+      </c>
+      <c r="B5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E5" t="s">
+        <v>238</v>
+      </c>
+      <c r="F5" t="s">
+        <v>239</v>
+      </c>
+      <c r="G5" t="s">
+        <v>240</v>
+      </c>
+      <c r="I5" t="s">
+        <v>241</v>
+      </c>
+      <c r="J5" t="s">
+        <v>242</v>
+      </c>
+      <c r="K5" t="s">
+        <v>243</v>
+      </c>
+      <c r="L5" t="s">
+        <v>244</v>
+      </c>
+      <c r="M5" t="s">
+        <v>243</v>
+      </c>
+      <c r="N5" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added old tokenizer for bert-base thai.
</commit_message>
<xml_diff>
--- a/output/DEEP_BASE.xlsx
+++ b/output/DEEP_BASE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pree\Thai_SA_journal\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B60B41-C3D6-424B-BC3A-2A714E433142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E306929-D064-49A5-97EF-5F03E54354B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WS" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="258">
   <si>
     <t>0RF</t>
   </si>
@@ -464,9 +464,6 @@
     <t>CNN</t>
   </si>
   <si>
-    <t>BERT</t>
-  </si>
-  <si>
     <t>Bi-LSTM</t>
   </si>
   <si>
@@ -746,9 +743,6 @@
     <t>0.6339±0.0385</t>
   </si>
   <si>
-    <t>BERT-MULT</t>
-  </si>
-  <si>
     <t>0.6305±0.015</t>
   </si>
   <si>
@@ -774,6 +768,48 @@
   </si>
   <si>
     <t>0.578±0.0258</t>
+  </si>
+  <si>
+    <t>BERT-MULTI</t>
+  </si>
+  <si>
+    <t>0.6165±0.0113</t>
+  </si>
+  <si>
+    <t>0.6792±0.0125</t>
+  </si>
+  <si>
+    <t>0.5224±0.0124</t>
+  </si>
+  <si>
+    <t>0.3065±0.0299</t>
+  </si>
+  <si>
+    <t>0.8578±0.006</t>
+  </si>
+  <si>
+    <t>0.3782±0.0265</t>
+  </si>
+  <si>
+    <t>0.6083±0.0125</t>
+  </si>
+  <si>
+    <t>0.5151±0.0861</t>
+  </si>
+  <si>
+    <t>0.3561±0.027</t>
+  </si>
+  <si>
+    <t>0.2786±0.0355</t>
+  </si>
+  <si>
+    <t>0.5708±0.018</t>
+  </si>
+  <si>
+    <t>0.4194±0.0404</t>
+  </si>
+  <si>
+    <t>BERT-THAI</t>
   </si>
 </sst>
 </file>
@@ -1653,12 +1689,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D5C4ABC-024F-46B2-BF47-2362A367FE2E}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="14" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1713,90 +1750,128 @@
         <v>141</v>
       </c>
       <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" t="s">
         <v>144</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>145</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>146</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>147</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>148</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>149</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>150</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>151</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>152</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>153</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>154</v>
-      </c>
-      <c r="N3" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4" t="s">
         <v>204</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>205</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>206</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>207</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>208</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>209</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>210</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>211</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>212</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>213</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>214</v>
-      </c>
-      <c r="N4" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
-        <v>142</v>
+        <v>244</v>
+      </c>
+      <c r="B5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D5" t="s">
+        <v>247</v>
+      </c>
+      <c r="E5" t="s">
+        <v>248</v>
+      </c>
+      <c r="F5" t="s">
+        <v>249</v>
+      </c>
+      <c r="G5" t="s">
+        <v>250</v>
+      </c>
+      <c r="I5" t="s">
+        <v>251</v>
+      </c>
+      <c r="J5" t="s">
+        <v>252</v>
+      </c>
+      <c r="K5" t="s">
+        <v>253</v>
+      </c>
+      <c r="L5" t="s">
+        <v>254</v>
+      </c>
+      <c r="M5" t="s">
+        <v>255</v>
+      </c>
+      <c r="N5" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1"/>
@@ -1832,11 +1907,12 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="14" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1891,90 +1967,92 @@
         <v>141</v>
       </c>
       <c r="B3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" t="s">
         <v>168</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>169</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>170</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>171</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>172</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>173</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>174</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>175</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>176</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>177</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>178</v>
-      </c>
-      <c r="N3" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" t="s">
         <v>156</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>157</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>158</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>159</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>160</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>161</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>162</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>163</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>164</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>165</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>166</v>
-      </c>
-      <c r="N4" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
-        <v>142</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1"/>
@@ -2007,13 +2085,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19A0F0F-E513-4C34-BBE6-40C2E11D5D35}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="A1:N5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
@@ -2066,87 +2147,92 @@
         <v>141</v>
       </c>
       <c r="B3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" t="s">
         <v>180</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>181</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>182</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>183</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>184</v>
-      </c>
-      <c r="G3" t="s">
-        <v>185</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" t="s">
+        <v>185</v>
+      </c>
+      <c r="J3" t="s">
         <v>186</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>187</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>188</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>189</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>190</v>
-      </c>
-      <c r="N3" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" t="s">
         <v>192</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>193</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>194</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>195</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>196</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>197</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>198</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>199</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>200</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>201</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>202</v>
-      </c>
-      <c r="N4" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
-        <v>142</v>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -2156,10 +2242,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8EE0488-B36D-46E6-911B-C64CBA69DD12}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="A5:O5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2218,123 +2304,128 @@
         <v>141</v>
       </c>
       <c r="B3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D3" t="s">
+        <v>225</v>
+      </c>
+      <c r="E3" t="s">
         <v>226</v>
       </c>
-      <c r="C3" t="s">
-        <v>226</v>
-      </c>
-      <c r="D3" t="s">
-        <v>226</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>227</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>228</v>
-      </c>
-      <c r="G3" t="s">
-        <v>229</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" t="s">
+        <v>229</v>
+      </c>
+      <c r="J3" t="s">
         <v>230</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>231</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>232</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>233</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>234</v>
-      </c>
-      <c r="N3" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D4" t="s">
+        <v>215</v>
+      </c>
+      <c r="E4" t="s">
         <v>216</v>
       </c>
-      <c r="C4" t="s">
-        <v>216</v>
-      </c>
-      <c r="D4" t="s">
-        <v>216</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>217</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>218</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>219</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>220</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>221</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>222</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>223</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>224</v>
-      </c>
-      <c r="N4" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" t="s">
+        <v>235</v>
+      </c>
+      <c r="D5" t="s">
+        <v>235</v>
+      </c>
+      <c r="E5" t="s">
         <v>236</v>
       </c>
-      <c r="B5" t="s">
+      <c r="F5" t="s">
         <v>237</v>
       </c>
-      <c r="C5" t="s">
-        <v>237</v>
-      </c>
-      <c r="D5" t="s">
-        <v>237</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>238</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I5" t="s">
         <v>239</v>
       </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
         <v>240</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>241</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>242</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
+        <v>241</v>
+      </c>
+      <c r="N5" t="s">
         <v>243</v>
       </c>
-      <c r="L5" t="s">
-        <v>244</v>
-      </c>
-      <c r="M5" t="s">
-        <v>243</v>
-      </c>
-      <c r="N5" t="s">
-        <v>245</v>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added: BERT TT results.
</commit_message>
<xml_diff>
--- a/output/DEEP_BASE.xlsx
+++ b/output/DEEP_BASE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pree\Thai_SA_journal\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9102F7-D704-4684-8DF6-BA070BD96F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D30049-996D-481E-903F-02A4E298B8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="258">
   <si>
     <t>0SVMRBF</t>
   </si>
@@ -774,6 +774,42 @@
   </si>
   <si>
     <t>0.6441±0.0309</t>
+  </si>
+  <si>
+    <t>0.6791±0.0194</t>
+  </si>
+  <si>
+    <t>0.8732±0.1075</t>
+  </si>
+  <si>
+    <t>0.6682±0.0227</t>
+  </si>
+  <si>
+    <t>0.4926±0.0378</t>
+  </si>
+  <si>
+    <t>0.8208±0.0175</t>
+  </si>
+  <si>
+    <t>0.6571±0.0301</t>
+  </si>
+  <si>
+    <t>0.6567±0.0279</t>
+  </si>
+  <si>
+    <t>0.6489±0.0336</t>
+  </si>
+  <si>
+    <t>0.6315±0.0347</t>
+  </si>
+  <si>
+    <t>0.457±0.0447</t>
+  </si>
+  <si>
+    <t>0.7236±0.026</t>
+  </si>
+  <si>
+    <t>0.6399±0.0322</t>
   </si>
 </sst>
 </file>
@@ -1510,7 +1546,9 @@
   </sheetPr>
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5:N5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1666,19 +1704,43 @@
       <c r="A5" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="B5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C5" t="s">
+        <v>247</v>
+      </c>
+      <c r="D5" t="s">
+        <v>248</v>
+      </c>
+      <c r="E5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F5" t="s">
+        <v>250</v>
+      </c>
+      <c r="G5" t="s">
+        <v>251</v>
+      </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
+      <c r="I5" t="s">
+        <v>252</v>
+      </c>
+      <c r="J5" t="s">
+        <v>253</v>
+      </c>
+      <c r="K5" t="s">
+        <v>254</v>
+      </c>
+      <c r="L5" t="s">
+        <v>255</v>
+      </c>
+      <c r="M5" t="s">
+        <v>256</v>
+      </c>
+      <c r="N5" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
@@ -2038,8 +2100,8 @@
   </sheetPr>
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added: BERT KT result.
</commit_message>
<xml_diff>
--- a/output/DEEP_BASE.xlsx
+++ b/output/DEEP_BASE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pree\Thai_SA_journal\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D1C03A-B734-4DED-81F6-D30261553EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED59C07-DE6A-4837-8568-C20EC7C8B08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="283">
   <si>
     <t>0SVMRBF</t>
   </si>
@@ -635,9 +635,6 @@
     <t>0.636±0.0061</t>
   </si>
   <si>
-    <t xml:space="preserve"> ml =50 , lr=5e-5 ep = 10     bs = 140</t>
-  </si>
-  <si>
     <t>0.5198±0.0226</t>
   </si>
   <si>
@@ -852,6 +849,42 @@
   </si>
   <si>
     <t>0.5544±0.0231</t>
+  </si>
+  <si>
+    <t>0.7786±0.003</t>
+  </si>
+  <si>
+    <t>0.7881±0.003</t>
+  </si>
+  <si>
+    <t>0.7686±0.0053</t>
+  </si>
+  <si>
+    <t>0.5651±0.0051</t>
+  </si>
+  <si>
+    <t>0.9181±0.0021</t>
+  </si>
+  <si>
+    <t>0.7127±0.0048</t>
+  </si>
+  <si>
+    <t>0.7721±0.007</t>
+  </si>
+  <si>
+    <t>0.7362±0.0185</t>
+  </si>
+  <si>
+    <t>0.6851±0.0228</t>
+  </si>
+  <si>
+    <t>0.5553±0.0128</t>
+  </si>
+  <si>
+    <t>0.7638±0.0171</t>
+  </si>
+  <si>
+    <t>0.7092±0.0081</t>
   </si>
 </sst>
 </file>
@@ -1278,8 +1311,8 @@
   </sheetPr>
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:N5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,41 +1386,41 @@
         <v>141</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1395,41 +1428,41 @@
         <v>152</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1437,41 +1470,41 @@
         <v>163</v>
       </c>
       <c r="B5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C5" t="s">
         <v>260</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>261</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>262</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>263</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>264</v>
-      </c>
-      <c r="G5" t="s">
-        <v>265</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
+        <v>265</v>
+      </c>
+      <c r="J5" t="s">
         <v>266</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>267</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>268</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>269</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>270</v>
-      </c>
-      <c r="N5" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1705,41 +1738,41 @@
         <v>141</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1747,41 +1780,41 @@
         <v>152</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1789,41 +1822,41 @@
         <v>163</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1984,7 +2017,9 @@
   </sheetPr>
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2142,21 +2177,43 @@
       <c r="A5" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
+      <c r="B5" t="s">
+        <v>271</v>
+      </c>
+      <c r="C5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D5" t="s">
+        <v>273</v>
+      </c>
+      <c r="E5" t="s">
+        <v>274</v>
+      </c>
+      <c r="F5" t="s">
+        <v>275</v>
+      </c>
+      <c r="G5" t="s">
+        <v>276</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" t="s">
+        <v>277</v>
+      </c>
+      <c r="J5" t="s">
+        <v>278</v>
+      </c>
+      <c r="K5" t="s">
+        <v>279</v>
+      </c>
+      <c r="L5" t="s">
+        <v>280</v>
+      </c>
+      <c r="M5" t="s">
+        <v>281</v>
+      </c>
+      <c r="N5" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="6" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">

</xml_diff>

<commit_message>
added: wangchan extracted results for TT, TX.
</commit_message>
<xml_diff>
--- a/output/DEEP_BASE.xlsx
+++ b/output/DEEP_BASE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pree\Thai_SA_journal\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2557AF6-2D5C-46A5-89C5-D20A44C10949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5315B6-C4D9-4CDD-989A-37534343F92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="309">
   <si>
     <t>0SVMRBF</t>
   </si>
@@ -885,6 +885,84 @@
   </si>
   <si>
     <t>WangchaRoberta</t>
+  </si>
+  <si>
+    <t>0.7679±0.0252</t>
+  </si>
+  <si>
+    <t>0.759±0.0283</t>
+  </si>
+  <si>
+    <t>0.7715±0.0199</t>
+  </si>
+  <si>
+    <t>0.6421±0.0351</t>
+  </si>
+  <si>
+    <t>0.9037±0.0097</t>
+  </si>
+  <si>
+    <t>0.7651±0.0232</t>
+  </si>
+  <si>
+    <t>0.7667±0.0288</t>
+  </si>
+  <si>
+    <t>0.7594±0.0264</t>
+  </si>
+  <si>
+    <t>0.7758±0.0293</t>
+  </si>
+  <si>
+    <t>0.6419±0.0439</t>
+  </si>
+  <si>
+    <t>0.8982±0.0205</t>
+  </si>
+  <si>
+    <t>0.7675±0.0271</t>
+  </si>
+  <si>
+    <t>0.7746±0.0297</t>
+  </si>
+  <si>
+    <t>0.7611±0.0317</t>
+  </si>
+  <si>
+    <t>0.8021±0.0438</t>
+  </si>
+  <si>
+    <t>0.5511±0.0601</t>
+  </si>
+  <si>
+    <t>0.8502±0.0229</t>
+  </si>
+  <si>
+    <t>0.7805±0.0296</t>
+  </si>
+  <si>
+    <t>0.7732±0.0275</t>
+  </si>
+  <si>
+    <t>0.7505±0.0306</t>
+  </si>
+  <si>
+    <t>0.82±0.0301</t>
+  </si>
+  <si>
+    <t>0.5493±0.0547</t>
+  </si>
+  <si>
+    <t>0.853±0.0149</t>
+  </si>
+  <si>
+    <t>0.7834±0.0254</t>
+  </si>
+  <si>
+    <t>WC-Extract</t>
+  </si>
+  <si>
+    <t>WC-Extract-Blending</t>
   </si>
 </sst>
 </file>
@@ -1311,8 +1389,8 @@
   </sheetPr>
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1665,8 +1743,8 @@
   </sheetPr>
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1863,24 +1941,50 @@
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+        <v>307</v>
+      </c>
+      <c r="B6" t="s">
+        <v>283</v>
+      </c>
+      <c r="C6" t="s">
+        <v>284</v>
+      </c>
+      <c r="D6" t="s">
+        <v>285</v>
+      </c>
+      <c r="E6" t="s">
+        <v>286</v>
+      </c>
+      <c r="F6" t="s">
+        <v>287</v>
+      </c>
+      <c r="G6" t="s">
+        <v>288</v>
+      </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
+      <c r="I6" t="s">
+        <v>289</v>
+      </c>
+      <c r="J6" t="s">
+        <v>290</v>
+      </c>
+      <c r="K6" t="s">
+        <v>291</v>
+      </c>
+      <c r="L6" t="s">
+        <v>292</v>
+      </c>
+      <c r="M6" t="s">
+        <v>293</v>
+      </c>
+      <c r="N6" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="9" t="s">
+        <v>308</v>
+      </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -2245,10 +2349,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2445,21 +2549,50 @@
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+        <v>307</v>
+      </c>
+      <c r="B6" t="s">
+        <v>295</v>
+      </c>
+      <c r="C6" t="s">
+        <v>296</v>
+      </c>
+      <c r="D6" t="s">
+        <v>297</v>
+      </c>
+      <c r="E6" t="s">
+        <v>298</v>
+      </c>
+      <c r="F6" t="s">
+        <v>299</v>
+      </c>
+      <c r="G6" t="s">
+        <v>300</v>
+      </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
+      <c r="I6" t="s">
+        <v>301</v>
+      </c>
+      <c r="J6" t="s">
+        <v>302</v>
+      </c>
+      <c r="K6" t="s">
+        <v>303</v>
+      </c>
+      <c r="L6" t="s">
+        <v>304</v>
+      </c>
+      <c r="M6" t="s">
+        <v>305</v>
+      </c>
+      <c r="N6" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>308</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2473,7 +2606,7 @@
   </sheetPr>
   <dimension ref="A1:AD120"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
completed deep base line results.
</commit_message>
<xml_diff>
--- a/output/DEEP_BASE.xlsx
+++ b/output/DEEP_BASE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pree\Thai_SA_journal\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA30D825-56A4-4847-9405-FE991E247A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BE2282-C42A-4121-89E8-CBAF4121637F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="331">
   <si>
     <t>0SVMRBF</t>
   </si>
@@ -884,9 +884,6 @@
     <t>0.7092±0.0081</t>
   </si>
   <si>
-    <t>WangchaRoberta</t>
-  </si>
-  <si>
     <t>0.7746±0.0297</t>
   </si>
   <si>
@@ -926,9 +923,6 @@
     <t>WC-Extract</t>
   </si>
   <si>
-    <t>WC-Extract-Blending</t>
-  </si>
-  <si>
     <t>0.7679±0.0197</t>
   </si>
   <si>
@@ -963,6 +957,78 @@
   </si>
   <si>
     <t>0.7669±0.0288</t>
+  </si>
+  <si>
+    <t>0.7348±0.0182</t>
+  </si>
+  <si>
+    <t>0.675±0.0281</t>
+  </si>
+  <si>
+    <t>0.5787±0.0359</t>
+  </si>
+  <si>
+    <t>0.5499±0.0352</t>
+  </si>
+  <si>
+    <t>0.866±0.0154</t>
+  </si>
+  <si>
+    <t>0.6222±0.0225</t>
+  </si>
+  <si>
+    <t>0.7341±0.0153</t>
+  </si>
+  <si>
+    <t>0.679±0.0218</t>
+  </si>
+  <si>
+    <t>0.5777±0.0348</t>
+  </si>
+  <si>
+    <t>0.548±0.0292</t>
+  </si>
+  <si>
+    <t>0.8654±0.0153</t>
+  </si>
+  <si>
+    <t>0.6235±0.0199</t>
+  </si>
+  <si>
+    <t>0.8153±0.0334</t>
+  </si>
+  <si>
+    <t>0.7862±0.0287</t>
+  </si>
+  <si>
+    <t>0.7594±0.0699</t>
+  </si>
+  <si>
+    <t>0.6439±0.0772</t>
+  </si>
+  <si>
+    <t>0.9064±0.0309</t>
+  </si>
+  <si>
+    <t>0.7719±0.0499</t>
+  </si>
+  <si>
+    <t>0.8149±0.0344</t>
+  </si>
+  <si>
+    <t>0.787±0.0302</t>
+  </si>
+  <si>
+    <t>0.7565±0.0711</t>
+  </si>
+  <si>
+    <t>0.6423±0.0791</t>
+  </si>
+  <si>
+    <t>0.9047±0.0317</t>
+  </si>
+  <si>
+    <t>0.7707±0.051</t>
   </si>
 </sst>
 </file>
@@ -1390,7 +1456,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1587,21 +1653,45 @@
     </row>
     <row r="6" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+        <v>294</v>
+      </c>
+      <c r="B6" t="s">
+        <v>307</v>
+      </c>
+      <c r="C6" t="s">
+        <v>308</v>
+      </c>
+      <c r="D6" t="s">
+        <v>309</v>
+      </c>
+      <c r="E6" t="s">
+        <v>310</v>
+      </c>
+      <c r="F6" t="s">
+        <v>311</v>
+      </c>
+      <c r="G6" t="s">
+        <v>312</v>
+      </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
+      <c r="I6" t="s">
+        <v>313</v>
+      </c>
+      <c r="J6" t="s">
+        <v>314</v>
+      </c>
+      <c r="K6" t="s">
+        <v>315</v>
+      </c>
+      <c r="L6" t="s">
+        <v>316</v>
+      </c>
+      <c r="M6" t="s">
+        <v>317</v>
+      </c>
+      <c r="N6" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="7" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
@@ -1741,10 +1831,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:N6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1941,50 +2031,48 @@
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="B6" t="s">
         <v>295</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>296</v>
+      </c>
+      <c r="D6" t="s">
         <v>297</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>298</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>299</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>300</v>
-      </c>
-      <c r="F6" t="s">
-        <v>301</v>
-      </c>
-      <c r="G6" t="s">
-        <v>302</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
+        <v>301</v>
+      </c>
+      <c r="J6" t="s">
+        <v>302</v>
+      </c>
+      <c r="K6" t="s">
         <v>303</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>304</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>305</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>306</v>
       </c>
-      <c r="M6" t="s">
-        <v>307</v>
-      </c>
-      <c r="N6" t="s">
-        <v>308</v>
-      </c>
     </row>
     <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>296</v>
-      </c>
+      <c r="A7" s="9"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -2095,22 +2183,6 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2123,8 +2195,8 @@
   </sheetPr>
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2323,21 +2395,45 @@
     </row>
     <row r="6" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+        <v>294</v>
+      </c>
+      <c r="B6" t="s">
+        <v>319</v>
+      </c>
+      <c r="C6" t="s">
+        <v>320</v>
+      </c>
+      <c r="D6" t="s">
+        <v>321</v>
+      </c>
+      <c r="E6" t="s">
+        <v>322</v>
+      </c>
+      <c r="F6" t="s">
+        <v>323</v>
+      </c>
+      <c r="G6" t="s">
+        <v>324</v>
+      </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
+      <c r="I6" t="s">
+        <v>325</v>
+      </c>
+      <c r="J6" t="s">
+        <v>326</v>
+      </c>
+      <c r="K6" t="s">
+        <v>327</v>
+      </c>
+      <c r="L6" t="s">
+        <v>328</v>
+      </c>
+      <c r="M6" t="s">
+        <v>329</v>
+      </c>
+      <c r="N6" t="s">
+        <v>330</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2349,10 +2445,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="I6:N6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2549,49 +2645,44 @@
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B6" t="s">
+        <v>282</v>
+      </c>
+      <c r="C6" t="s">
         <v>283</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>284</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>285</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>286</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>287</v>
-      </c>
-      <c r="G6" t="s">
-        <v>288</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
+        <v>288</v>
+      </c>
+      <c r="J6" t="s">
         <v>289</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>290</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>291</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>292</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>293</v>
-      </c>
-      <c r="N6" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated: add embedded config model yaml file.
</commit_message>
<xml_diff>
--- a/output/DEEP_BASE.xlsx
+++ b/output/DEEP_BASE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="WS"/>
@@ -614,40 +614,40 @@
     <t>0.6273±0.0063</t>
   </si>
   <si>
-    <t>0.7383±0.0037</t>
-  </si>
-  <si>
-    <t>0.7643±0.0042</t>
-  </si>
-  <si>
-    <t>0.7131±0.0032</t>
-  </si>
-  <si>
-    <t>0.4695±0.0061</t>
-  </si>
-  <si>
-    <t>0.888±0.0031</t>
-  </si>
-  <si>
-    <t>0.6361±0.0048</t>
-  </si>
-  <si>
-    <t>0.7306±0.0053</t>
-  </si>
-  <si>
-    <t>0.6725±0.0117</t>
-  </si>
-  <si>
-    <t>0.6035±0.008</t>
-  </si>
-  <si>
-    <t>0.4576±0.009</t>
-  </si>
-  <si>
-    <t>0.8254±0.0075</t>
-  </si>
-  <si>
-    <t>0.636±0.0061</t>
+    <t>0.7276±0.0041</t>
+  </si>
+  <si>
+    <t>0.667±0.0104</t>
+  </si>
+  <si>
+    <t>0.5938±0.0098</t>
+  </si>
+  <si>
+    <t>0.4493±0.0069</t>
+  </si>
+  <si>
+    <t>0.8212±0.0052</t>
+  </si>
+  <si>
+    <t>0.6281±0.0036</t>
+  </si>
+  <si>
+    <t>0.6988±0.0058</t>
+  </si>
+  <si>
+    <t>0.6199±0.0083</t>
+  </si>
+  <si>
+    <t>0.5928±0.0063</t>
+  </si>
+  <si>
+    <t>0.4117±0.0077</t>
+  </si>
+  <si>
+    <t>0.7803±0.0064</t>
+  </si>
+  <si>
+    <t>0.606±0.005</t>
   </si>
   <si>
     <t>0.7786±0.003</t>
@@ -1814,7 +1814,7 @@
   </sheetPr>
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2186,7 +2186,7 @@
   </sheetPr>
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>